<commit_message>
Updates and new sketch
</commit_message>
<xml_diff>
--- a/Shadow_Dave_MarcDuino_Warpdrives_UtilArms_2_0_Flithy_Body/Dave Shadow Sounds.xlsx
+++ b/Shadow_Dave_MarcDuino_Warpdrives_UtilArms_2_0_Flithy_Body/Dave Shadow Sounds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\David\Documents\GitHub\SHADOW\Shadow_Dave_MarcDuino_Warpdrives_UtilArms_2_0_Flithy_Body\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/89a0f6bfeb935e23/Documents/Git/Shadow/Shadow_Dave_MarcDuino_Warpdrives_UtilArms_2_0_Flithy_Body/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6065A2-C1C2-4CB4-9581-B0B9220BF9A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3B6065A2-C1C2-4CB4-9581-B0B9220BF9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A361D86-D282-401A-AFD6-4EC0873A9F2B}"/>
   <bookViews>
-    <workbookView xWindow="-5160" yWindow="672" windowWidth="10488" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,10 +188,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -229,9 +233,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,26 +268,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,26 +303,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -513,19 +483,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E2" sqref="E2"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>4</v>
       </c>
@@ -536,7 +506,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -553,7 +523,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -570,7 +540,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -587,7 +557,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -604,10 +574,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -624,7 +594,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -653,7 +623,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -665,7 +635,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>